<commit_message>
from Apex end of day Apr19 2018
</commit_message>
<xml_diff>
--- a/R/Data/analyst_alert_04192018.xlsx
+++ b/R/Data/analyst_alert_04192018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YChen\Documents\git\working_dir\R\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{836ACD8C-6264-451E-9D95-FF0DB9C43BA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{213C48F7-4A98-4F07-B7F1-E1AC3FC92CAC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10395" yWindow="-105" windowWidth="14850" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1656,13 +1656,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:XFD368"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3253,5 +3256,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>